<commit_message>
thay đổi docs week 2
thay đổi docs week 2
</commit_message>
<xml_diff>
--- a/ISP392/Week2/Docs/Project Tracking interation 1.xlsx
+++ b/ISP392/Week2/Docs/Project Tracking interation 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -64,57 +64,75 @@
     <t>Quang Tú</t>
   </si>
   <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Product Details</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Details like description, color, size, ... for customer to choose</t>
+  </si>
+  <si>
+    <t>Product list</t>
+  </si>
+  <si>
+    <t>Customer can see products that they have just searched</t>
+  </si>
+  <si>
+    <t>Cart Details</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>List of all the products that have been added into the cart</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>User will login with account</t>
+  </si>
+  <si>
+    <t>Đức Thái</t>
+  </si>
+  <si>
+    <t>User Register</t>
+  </si>
+  <si>
+    <t>Customer can register a new account here</t>
+  </si>
+  <si>
+    <t>User List</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Admin manage accounts</t>
+  </si>
+  <si>
+    <t>User Details</t>
+  </si>
+  <si>
+    <t>User can view information about account and update information</t>
+  </si>
+  <si>
     <t>Not Start</t>
   </si>
   <si>
-    <t>Product Details</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Details like description, color, size, ... for customer to choose</t>
-  </si>
-  <si>
-    <t>Cart Details</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Complex</t>
-  </si>
-  <si>
-    <t>List of all the products that have been added into the cart</t>
-  </si>
-  <si>
-    <t>User Login</t>
-  </si>
-  <si>
-    <t>Common</t>
-  </si>
-  <si>
-    <t>User will login with account</t>
-  </si>
-  <si>
-    <t>Đức Thái</t>
-  </si>
-  <si>
-    <t>User Register</t>
-  </si>
-  <si>
-    <t>Customer can register a new account here</t>
-  </si>
-  <si>
-    <t>User Details</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>User can view information about account and update information</t>
-  </si>
-  <si>
     <t>Reset Password</t>
   </si>
   <si>
@@ -133,12 +151,6 @@
     <t>It allow user can change new password</t>
   </si>
   <si>
-    <t>User List</t>
-  </si>
-  <si>
-    <t>Admin manage accounts</t>
-  </si>
-  <si>
     <t>Cart Completion (Place Order)</t>
   </si>
   <si>
@@ -184,7 +196,7 @@
     <t>User can view feedback from other customer about a product</t>
   </si>
   <si>
-    <t>literation 2</t>
+    <t>literation 1</t>
   </si>
 </sst>
 </file>
@@ -192,12 +204,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,20 +269,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="9"/>
       <name val="Sitka Display"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -305,9 +305,108 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -319,50 +418,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -371,25 +426,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,60 +447,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="41">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,19 +499,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,61 +661,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,103 +673,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,24 +784,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -849,32 +832,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -893,160 +850,184 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="28" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1087,52 +1068,49 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1459,10 +1437,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1532,7 +1510,7 @@
       <c r="H2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="24" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1559,7 +1537,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="11"/>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="24" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1571,13 +1549,13 @@
         <v>20</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>13</v>
@@ -1585,26 +1563,26 @@
       <c r="G4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="27" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="20.55" spans="1:9">
+    <row r="5" ht="40.35" spans="1:9">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>13</v>
@@ -1612,22 +1590,20 @@
       <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>16</v>
+      <c r="H5" s="13"/>
+      <c r="I5" s="25" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="6" ht="40.35" spans="1:9">
+    <row r="6" ht="20.55" spans="1:9">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>11</v>
@@ -1641,23 +1617,25 @@
       <c r="G6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="27" t="s">
+      <c r="H6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="60.15" spans="1:9">
+    <row r="7" ht="40.35" spans="1:9">
       <c r="A7" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>32</v>
@@ -1668,215 +1646,213 @@
       <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="27" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" ht="60.15" spans="1:9">
+    <row r="8" ht="20.55" spans="1:9">
       <c r="A8" s="5">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" ht="60.15" spans="1:9">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="27" t="s">
-        <v>16</v>
+      <c r="C9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="26" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="9" ht="40.35" spans="1:9">
-      <c r="A9" s="5">
+    <row r="10" ht="60.15" spans="1:9">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="27" t="s">
-        <v>16</v>
+      <c r="H10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="10" ht="20.55" spans="1:9">
-      <c r="A10" s="5">
+    <row r="11" ht="40.35" spans="1:9">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="B11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="D11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="27" t="s">
-        <v>16</v>
+      <c r="H11" s="17"/>
+      <c r="I11" s="25" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="11" ht="60.15" spans="1:9">
-      <c r="A11" s="5">
+    <row r="12" ht="60.15" spans="1:9">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" ht="40.35" spans="1:9">
-      <c r="A12" s="5">
-        <v>12</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>34</v>
+      <c r="B12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="28" t="s">
-        <v>16</v>
+      <c r="H12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" ht="40.35" spans="1:9">
       <c r="A13" s="5">
-        <v>13</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="28" t="s">
-        <v>16</v>
+      <c r="H13" s="11"/>
+      <c r="I13" s="27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" ht="40.35" spans="1:9">
       <c r="A14" s="5">
-        <v>14</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>16</v>
+      <c r="H14" s="13"/>
+      <c r="I14" s="27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" ht="40.35" spans="1:9">
-      <c r="A15" s="19">
-        <v>15</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>52</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>18</v>
@@ -1884,51 +1860,80 @@
       <c r="E15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="28" t="s">
-        <v>16</v>
+      <c r="H15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" ht="40.35" spans="1:9">
-      <c r="A16" s="21">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" ht="40.35" spans="1:9">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B17" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="26" t="s">
+      <c r="E17" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="29" t="s">
-        <v>16</v>
+      <c r="H17" s="13"/>
+      <c r="I17" s="28" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
thay đổi interation 1
</commit_message>
<xml_diff>
--- a/ISP392/Week2/Docs/Project Tracking interation 1.xlsx
+++ b/ISP392/Week2/Docs/Project Tracking interation 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -82,118 +82,79 @@
     <t>Customer can see products that they have just searched</t>
   </si>
   <si>
-    <t>Cart Details</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Complex</t>
-  </si>
-  <si>
-    <t>List of all the products that have been added into the cart</t>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>User will login with account</t>
+  </si>
+  <si>
+    <t>Đức Thái</t>
+  </si>
+  <si>
+    <t>User Register</t>
+  </si>
+  <si>
+    <t>Customer can register a new account here</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>User can retrieve password when forgotten by confirming information via email</t>
+  </si>
+  <si>
+    <t>Linh Trang</t>
   </si>
   <si>
     <t>In progress</t>
   </si>
   <si>
-    <t>User Login</t>
-  </si>
-  <si>
-    <t>Common</t>
-  </si>
-  <si>
-    <t>User will login with account</t>
-  </si>
-  <si>
-    <t>Đức Thái</t>
-  </si>
-  <si>
-    <t>User Register</t>
-  </si>
-  <si>
-    <t>Customer can register a new account here</t>
-  </si>
-  <si>
-    <t>User List</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Admin manage accounts</t>
-  </si>
-  <si>
-    <t>User Details</t>
-  </si>
-  <si>
-    <t>User can view information about account and update information</t>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>It allow user can change new password</t>
+  </si>
+  <si>
+    <t>Products List</t>
+  </si>
+  <si>
+    <t>Seller</t>
+  </si>
+  <si>
+    <t>seller views and manages all products</t>
+  </si>
+  <si>
+    <t>Xuân Thái</t>
   </si>
   <si>
     <t>Not Start</t>
   </si>
   <si>
-    <t>Reset Password</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>User can retrieve password when forgotten by confirming information via email</t>
-  </si>
-  <si>
-    <t>Linh Trang</t>
-  </si>
-  <si>
-    <t>Change Password</t>
-  </si>
-  <si>
-    <t>It allow user can change new password</t>
-  </si>
-  <si>
-    <t>Cart Completion (Place Order)</t>
-  </si>
-  <si>
-    <t>Customer can comfirm order information like shipping information,... or change it</t>
-  </si>
-  <si>
-    <t>Xuân Thái</t>
-  </si>
-  <si>
     <t>User Profile</t>
   </si>
   <si>
     <t>User can view and update user's infomation</t>
   </si>
   <si>
-    <t>My Orders (xem lịch sử order) (Tổng quát)</t>
-  </si>
-  <si>
-    <t>Customers can view history of orders</t>
-  </si>
-  <si>
-    <t>Order Details (chi tiết)</t>
-  </si>
-  <si>
-    <t>Seller views the detail of 1 of his orders</t>
+    <t>Blog Details</t>
+  </si>
+  <si>
+    <t>Content of a blog</t>
   </si>
   <si>
     <t>Ngọc Thành</t>
   </si>
   <si>
-    <t>Products List</t>
-  </si>
-  <si>
-    <t>Seller</t>
-  </si>
-  <si>
-    <t>seller views and manages all products</t>
-  </si>
-  <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>User can view feedback from other customer about a product</t>
+    <t>Blogs List</t>
+  </si>
+  <si>
+    <t>List of all the blogs for visitor to read</t>
   </si>
   <si>
     <t>literation 1</t>
@@ -205,9 +166,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -304,6 +265,36 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -311,10 +302,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -322,6 +337,45 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -333,88 +387,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -427,21 +403,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -511,174 +472,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -763,8 +724,8 @@
         <color rgb="FFCCCCCC"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -772,23 +733,25 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,17 +813,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -879,155 +844,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1065,21 +1039,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1098,13 +1078,13 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1437,10 +1417,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1510,7 +1490,7 @@
       <c r="H2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="27" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1537,7 +1517,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="11"/>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="27" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1564,11 +1544,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="40.35" spans="1:9">
+    <row r="5" ht="20.55" spans="1:9">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1578,11 +1558,11 @@
       <c r="C5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>13</v>
@@ -1590,26 +1570,28 @@
       <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="25" t="s">
-        <v>26</v>
+      <c r="H5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" ht="20.55" spans="1:9">
+    <row r="6" ht="40.35" spans="1:9">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>13</v>
@@ -1617,28 +1599,26 @@
       <c r="G6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="24" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="40.35" spans="1:9">
+    <row r="7" ht="60.15" spans="1:9">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>13</v>
@@ -1646,47 +1626,49 @@
       <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="24" t="s">
-        <v>16</v>
+      <c r="H7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="8" ht="20.55" spans="1:9">
+    <row r="8" ht="40.35" spans="1:9">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="25" t="s">
-        <v>26</v>
+      <c r="H8" s="18"/>
+      <c r="I8" s="28" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="9" ht="60.15" spans="1:9">
+    <row r="9" ht="40.35" spans="1:9">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>18</v>
@@ -1694,246 +1676,109 @@
       <c r="E9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="26" t="s">
+      <c r="H9" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="I9" s="29" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="10" ht="60.15" spans="1:9">
+    <row r="10" ht="40.35" spans="1:9">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="16" t="s">
         <v>40</v>
       </c>
+      <c r="C10" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>26</v>
+      <c r="H10" s="19"/>
+      <c r="I10" s="29" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="11" ht="40.35" spans="1:9">
+    <row r="11" ht="20.55" spans="1:9">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>40</v>
+      <c r="B11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="25" t="s">
-        <v>26</v>
+      <c r="I11" s="29" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="12" ht="60.15" spans="1:9">
+    <row r="12" ht="40.35" spans="1:9">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="C12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="15" t="s">
+      <c r="F12" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" ht="40.35" spans="1:9">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" ht="40.35" spans="1:9">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" ht="40.35" spans="1:9">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" ht="40.35" spans="1:9">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" ht="40.35" spans="1:9">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="28" t="s">
-        <v>38</v>
+      <c r="H12" s="26"/>
+      <c r="I12" s="30" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>